<commit_message>
gestion de la lecture de la base de données
</commit_message>
<xml_diff>
--- a/src/loader_package/xlsx/big_pre_load.xlsx
+++ b/src/loader_package/xlsx/big_pre_load.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\java_project_desautel_pellen_perold\src\loader_package\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E17619B-7934-4880-A880-21130550D762}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E635C908-AED9-490E-A43E-DC5DDD93235F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,6 +19,9 @@
     <sheet name="official" sheetId="4" r:id="rId4"/>
     <sheet name="election" sheetId="5" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">elector!$E$1:$E$1001</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -6132,7 +6135,7 @@
   <dimension ref="A1:F1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6162,7 +6165,7 @@
         <v>1906</v>
       </c>
       <c r="F1" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>